<commit_message>
add cost of oscillator and synthesizer to BOM
they were not quoted in Advanced Assembly's due to MOQ issue
</commit_message>
<xml_diff>
--- a/manufacture/rasdr2-bom-and-components.xlsx
+++ b/manufacture/rasdr2-bom-and-components.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="3195" yWindow="0" windowWidth="19320" windowHeight="15480" tabRatio="500"/>
+    <workbookView xWindow="3195" yWindow="0" windowWidth="19320" windowHeight="13740" tabRatio="500" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="CostPerUnit" sheetId="7" r:id="rId1"/>
@@ -488,7 +488,18 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:spPr>
+            <a:ln w="38100"/>
+          </c:spPr>
+          <c:marker>
+            <c:spPr>
+              <a:ln w="38100"/>
+            </c:spPr>
+          </c:marker>
           <c:trendline>
+            <c:spPr>
+              <a:ln w="38100"/>
+            </c:spPr>
             <c:trendlineType val="power"/>
             <c:forward val="900"/>
             <c:backward val="5"/>
@@ -529,13 +540,13 @@
                 <c:formatCode>"$"#,##0.00_);[Red]\("$"#,##0.00\)</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>382.92455469534048</c:v>
+                  <c:v>412.57</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>640.18299999999999</c:v>
+                  <c:v>745.29</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>985.73779999999999</c:v>
+                  <c:v>1241.01</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -550,11 +561,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="75901184"/>
-        <c:axId val="75948032"/>
+        <c:axId val="34202752"/>
+        <c:axId val="34204288"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="75901184"/>
+        <c:axId val="34202752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="120"/>
@@ -565,12 +576,22 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="75948032"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="1"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="34204288"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="75948032"/>
+        <c:axId val="34204288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -581,7 +602,17 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="75901184"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="1"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="34202752"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -659,7 +690,18 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:spPr>
+            <a:ln w="38100"/>
+          </c:spPr>
+          <c:marker>
+            <c:spPr>
+              <a:ln w="38100"/>
+            </c:spPr>
+          </c:marker>
           <c:trendline>
+            <c:spPr>
+              <a:ln w="38100"/>
+            </c:spPr>
             <c:trendlineType val="power"/>
             <c:forward val="900"/>
             <c:backward val="5"/>
@@ -673,6 +715,16 @@
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:txPr>
+                <a:bodyPr/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="1400" b="1"/>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
             </c:trendlineLbl>
           </c:trendline>
           <c:xVal>
@@ -700,13 +752,13 @@
                 <c:formatCode>"$"#,##0.00_);[Red]\("$"#,##0.00\)</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>382.92455469534048</c:v>
+                  <c:v>412.57</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>640.18299999999999</c:v>
+                  <c:v>745.29</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>985.73779999999999</c:v>
+                  <c:v>1241.01</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -721,11 +773,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="120358016"/>
-        <c:axId val="76080256"/>
+        <c:axId val="153096192"/>
+        <c:axId val="153097728"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="120358016"/>
+        <c:axId val="153096192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1000"/>
@@ -736,12 +788,22 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="76080256"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="1"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="153097728"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="76080256"/>
+        <c:axId val="153097728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -752,7 +814,17 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="120358016"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="1"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="153096192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -761,6 +833,16 @@
       <c:legendPos val="r"/>
       <c:layout/>
       <c:overlay val="0"/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr b="1"/>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
@@ -773,7 +855,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="119" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="98" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
@@ -785,7 +867,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="119" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="98" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
@@ -797,7 +879,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8668550" cy="6291303"/>
+    <xdr:ext cx="8669694" cy="6288444"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>
@@ -824,7 +906,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8668550" cy="6291303"/>
+    <xdr:ext cx="8669694" cy="6288444"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>
@@ -1177,6 +1259,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="2" max="2" width="9.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1196,11 +1279,11 @@
         <v>100</v>
       </c>
       <c r="B2" s="3">
-        <v>382.92455469534048</v>
+        <v>412.57</v>
       </c>
       <c r="C2" s="3">
         <f>A2*B2</f>
-        <v>38292.455469534048</v>
+        <v>41257</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -1208,11 +1291,11 @@
         <v>25</v>
       </c>
       <c r="B3" s="3">
-        <v>640.18299999999999</v>
+        <v>745.29</v>
       </c>
       <c r="C3" s="3">
         <f>A3*B3</f>
-        <v>16004.575000000001</v>
+        <v>18632.25</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -1220,11 +1303,11 @@
         <v>10</v>
       </c>
       <c r="B4" s="3">
-        <v>985.73779999999999</v>
+        <v>1241.01</v>
       </c>
       <c r="C4" s="3">
         <f>A4*B4</f>
-        <v>9857.3780000000006</v>
+        <v>12410.1</v>
       </c>
     </row>
   </sheetData>
@@ -1951,19 +2034,19 @@
       </c>
       <c r="J18" s="4"/>
       <c r="K18" s="2">
-        <f>13285.81</f>
-        <v>13285.81</v>
+        <f>13285.81+(2500)+(100*4.65)</f>
+        <v>16250.81</v>
       </c>
       <c r="N18">
         <v>1</v>
       </c>
       <c r="O18" s="3">
         <f t="shared" si="8"/>
-        <v>132.85810000000001</v>
+        <v>162.50809999999998</v>
       </c>
       <c r="P18" s="3">
         <f t="shared" si="9"/>
-        <v>137.00809999999998</v>
+        <v>166.65809999999999</v>
       </c>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
@@ -2024,7 +2107,7 @@
       </c>
       <c r="P22" s="7">
         <f>SUM(P2:P19)</f>
-        <v>382.92455469534048</v>
+        <v>412.57455469534051</v>
       </c>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.25">
@@ -2091,8 +2174,8 @@
   </sheetPr>
   <dimension ref="A1:P39"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="P22" sqref="P22"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2801,18 +2884,19 @@
       </c>
       <c r="J18" s="4"/>
       <c r="K18" s="2">
-        <v>5656.76</v>
+        <f>5656.76+(2500)+(25*5.11)</f>
+        <v>8284.51</v>
       </c>
       <c r="N18">
         <v>1</v>
       </c>
       <c r="O18" s="3">
         <f t="shared" si="7"/>
-        <v>226.2704</v>
+        <v>331.38040000000001</v>
       </c>
       <c r="P18" s="3">
         <f t="shared" si="8"/>
-        <v>242.87040000000002</v>
+        <v>347.98040000000003</v>
       </c>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
@@ -2873,7 +2957,7 @@
       </c>
       <c r="P22" s="7">
         <f>SUM(P2:P19)</f>
-        <v>640.18299999999999</v>
+        <v>745.29300000000012</v>
       </c>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.25">
@@ -2942,7 +3026,7 @@
   <dimension ref="A1:P39"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="P18" sqref="P18:P19"/>
+      <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3468,7 +3552,7 @@
       </c>
       <c r="K13" s="2"/>
       <c r="O13" s="3">
-        <f t="shared" ref="O12:O14" si="6">SUM(I13:L13)/E13</f>
+        <f t="shared" ref="O13:O14" si="6">SUM(I13:L13)/E13</f>
         <v>3.9579999999999997</v>
       </c>
       <c r="P13" s="3">
@@ -3651,19 +3735,19 @@
       </c>
       <c r="J18" s="4"/>
       <c r="K18" s="2">
-        <f>3566.64</f>
-        <v>3566.64</v>
+        <f>3566.64+(2500)+(10*5.27)</f>
+        <v>6119.3399999999992</v>
       </c>
       <c r="N18">
         <v>1</v>
       </c>
       <c r="O18" s="3">
         <f t="shared" si="8"/>
-        <v>356.66399999999999</v>
+        <v>611.93399999999997</v>
       </c>
       <c r="P18" s="3">
-        <f t="shared" si="9"/>
-        <v>398.16399999999999</v>
+        <f>(SUM(H18:L18)/E18)*N18</f>
+        <v>653.43399999999997</v>
       </c>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
@@ -3724,7 +3808,7 @@
       </c>
       <c r="P22" s="7">
         <f>SUM(P2:P19)</f>
-        <v>985.73779999999999</v>
+        <v>1241.0077999999999</v>
       </c>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.25">

</xml_diff>